<commit_message>
general knowledge table update
</commit_message>
<xml_diff>
--- a/data/food_drink_trivia_correct_answers.xlsx
+++ b/data/food_drink_trivia_correct_answers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/Trivia/food_drink_trivia/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D69CA12-1416-B640-B782-418A7D728BEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18333E21-AAC3-7746-85BE-4BE3E54E8084}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16260" xr2:uid="{0F0A799C-CF3B-034E-811A-0FB1E9DFEA95}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>Movie Title</t>
   </si>
@@ -189,6 +189,36 @@
   </si>
   <si>
     <t>General Knowledge</t>
+  </si>
+  <si>
+    <t>What is Joey Chesnutt's record for most hot dogs eaten in a ten minute period?</t>
+  </si>
+  <si>
+    <t>What U.S. city has the most breweries per capita?</t>
+  </si>
+  <si>
+    <t>What is the most widely produced crop in the world?</t>
+  </si>
+  <si>
+    <t>How many Goldfish Crackers are in one serving?</t>
+  </si>
+  <si>
+    <t>What ingredient gives Malört</t>
+  </si>
+  <si>
+    <t>What is the scale used to measure the spice level of peppers?</t>
+  </si>
+  <si>
+    <t>What is the oldest brewery in the United States?</t>
+  </si>
+  <si>
+    <t>How many gallons of water does it take to make a 1/3 pound hamburger?</t>
+  </si>
+  <si>
+    <t>What are the five flavors of an original Rainbow Cone?</t>
+  </si>
+  <si>
+    <t>How many ingredients are in a Manhattan (including the garnish)?</t>
   </si>
 </sst>
 </file>
@@ -545,8 +575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01EF84FE-CF3D-2B40-A51D-56DFA01C7127}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18.83203125" defaultRowHeight="16"/>
@@ -580,15 +610,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="17">
+    <row r="2" spans="1:8" ht="85">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1">
-        <v>1</v>
+      <c r="D2" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="E2" s="1">
         <v>75</v>
@@ -603,7 +633,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="34">
+    <row r="3" spans="1:8" ht="51">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -613,8 +643,8 @@
       <c r="C3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="1">
-        <v>2</v>
+      <c r="D3" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>45</v>
@@ -629,7 +659,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="34">
+    <row r="4" spans="1:8" ht="51">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -639,8 +669,8 @@
       <c r="C4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="1">
-        <v>3</v>
+      <c r="D4" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>46</v>
@@ -655,7 +685,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="34">
+    <row r="5" spans="1:8" ht="51">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -665,8 +695,8 @@
       <c r="C5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="1">
-        <v>4</v>
+      <c r="D5" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="E5" s="1">
         <v>55</v>
@@ -691,8 +721,8 @@
       <c r="C6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="1">
-        <v>5</v>
+      <c r="D6" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>47</v>
@@ -707,7 +737,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="17">
+    <row r="7" spans="1:8" ht="68">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -717,8 +747,8 @@
       <c r="C7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="1">
-        <v>6</v>
+      <c r="D7" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>48</v>
@@ -733,7 +763,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="17">
+    <row r="8" spans="1:8" ht="51">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -743,8 +773,8 @@
       <c r="C8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="1">
-        <v>7</v>
+      <c r="D8" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>49</v>
@@ -759,7 +789,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="17">
+    <row r="9" spans="1:8" ht="68">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -769,8 +799,8 @@
       <c r="C9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="1">
-        <v>8</v>
+      <c r="D9" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="E9" s="1">
         <v>660</v>
@@ -795,8 +825,8 @@
       <c r="C10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="1">
-        <v>9</v>
+      <c r="D10" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>50</v>
@@ -811,7 +841,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="17">
+    <row r="11" spans="1:8" ht="68">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -821,8 +851,8 @@
       <c r="C11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="1">
-        <v>10</v>
+      <c r="D11" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="E11" s="1">
         <v>4</v>

</xml_diff>